<commit_message>
excel upload fixed reg no and student_ teacher swapped
</commit_message>
<xml_diff>
--- a/app/static/uploads/imgs/student_teacher_template_4.xlsx
+++ b/app/static/uploads/imgs/student_teacher_template_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JJ\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC498253-ECAE-478B-B618-DB7DCD238312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCE639-AD77-48FC-804D-B64DFFF4B35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students Template" sheetId="1" r:id="rId1"/>
@@ -21,14 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
-  <si>
-    <t>student_teacher</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>reg no</t>
   </si>
   <si>
+    <t xml:space="preserve"> student_teacher</t>
+  </si>
+  <si>
     <t>Semester</t>
   </si>
   <si>
@@ -44,7 +44,7 @@
     <t>Study Year</t>
   </si>
   <si>
-    <t>Terms</t>
+    <t>terms</t>
   </si>
   <si>
     <t>Schools</t>
@@ -56,61 +56,40 @@
     <t>study_year</t>
   </si>
   <si>
-    <t>Semester 1, Semester 2, Semester 3</t>
-  </si>
-  <si>
-    <t>Bachelor in Pre-Primary Education, Business Administration 12, Computer Science</t>
+    <t>Semester 1, Semester 2</t>
+  </si>
+  <si>
+    <t>Bachelor in Pre-Primary Education, BPPE, BTEC, Diploma in Pre-Primary Education, PGDE</t>
   </si>
   <si>
     <t>Hilton High, Mengo Senoir School, St. Bruno Sserunkuuma's SS</t>
   </si>
   <si>
-    <t>2024-2025, 2024/2025</t>
-  </si>
-  <si>
-    <t>year 1, year 2</t>
-  </si>
-  <si>
-    <t>kisaakye frank</t>
-  </si>
-  <si>
-    <t>12/u/1999</t>
+    <t>2022/2023, 2024/2025, 2025/2026</t>
+  </si>
+  <si>
+    <t>year 1, year 2, year 3</t>
+  </si>
+  <si>
+    <t>WALUIMBI ISIAH</t>
   </si>
   <si>
     <t>Semester 1</t>
   </si>
   <si>
-    <t>Hilton High</t>
-  </si>
-  <si>
-    <t>Business Administration 12</t>
-  </si>
-  <si>
-    <t>2024-2025</t>
+    <t>Mengo Senoir School</t>
+  </si>
+  <si>
+    <t>Bachelor in Pre-Primary Education</t>
+  </si>
+  <si>
+    <t>2022/2023</t>
   </si>
   <si>
     <t>year 1</t>
   </si>
   <si>
-    <t>Tamale Trevor</t>
-  </si>
-  <si>
-    <t>12/u/19991</t>
-  </si>
-  <si>
-    <t>Mengo Senoir School</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>12/u/1999101</t>
-  </si>
-  <si>
-    <t>12/u/19</t>
-  </si>
-  <si>
-    <t>12/u/19223</t>
+    <t>18/U/IE/178994589/PE</t>
   </si>
 </sst>
 </file>
@@ -450,18 +429,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="5" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -489,135 +467,43 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" sqref="C2:C100" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Semester 1,Semester 2,Semester 3"</formula1>
+      <formula1>"Semester 1,Semester 2"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E2:E100" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>"Bachelor in Pre-Primary Education,Business Administration 12,Computer Science"</formula1>
+      <formula1>"Bachelor in Pre-Primary Education,BPPE,BTEC,Diploma in Pre-Primary Education,PGDE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D2:D100" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hilton High,Mengo Senoir School,St. Bruno Sserunkuuma's SS"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="F2:F100" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>"2024-2025,2024/2025"</formula1>
+      <formula1>"2022/2023,2024/2025,2025/2026"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="G2:G100" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>"year 1,year 2"</formula1>
+      <formula1>"year 1,year 2,year 3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>